<commit_message>
feat: enhance writeField method to concatenate string values in NewExcelGenerator
</commit_message>
<xml_diff>
--- a/public/workbook-template.xlsx
+++ b/public/workbook-template.xlsx
@@ -17,10 +17,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1771276201" val="1228" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1771276201" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1771276201" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1771276201"/>
+      <pm:revision xmlns:pm="smNativeData" day="1771280302" val="1228" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1771280302" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1771280302" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1771280302"/>
     </ext>
   </extLst>
 </workbook>
@@ -32,7 +32,7 @@
     <t xml:space="preserve">Company Name: </t>
   </si>
   <si>
-    <t xml:space="preserve">Tax Period: </t>
+    <t xml:space="preserve">Workbook's Data Last Updated Tax Period: </t>
   </si>
   <si>
     <t>Financial Year:</t>
@@ -181,7 +181,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1771276201" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1771280302" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -196,7 +196,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1771276201" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1771280302" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -212,7 +212,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1771276201" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1771280302" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="200" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="200" lang="default" weight="bold"/>
@@ -228,7 +228,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1771276201" fgClr="FFFFFF" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1771280302" fgClr="FFFFFF" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="200" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="200" lang="default" weight="bold"/>
@@ -243,7 +243,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1771276201" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1771280302" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -252,7 +252,7 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,13 +265,24 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1771276201" type="1" fgLvl="100" fgClr="000070C0" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1771280302" type="1" fgLvl="100" fgClr="000070C0" bgLvl="0" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1771280302" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -287,7 +298,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1771276201"/>
+          <pm:border xmlns:pm="smNativeData" id="1771280302"/>
         </ext>
       </extLst>
     </border>
@@ -306,7 +317,26 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1771276201"/>
+          <pm:border xmlns:pm="smNativeData" id="1771280302"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1771280302"/>
         </ext>
       </extLst>
     </border>
@@ -329,10 +359,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1771276201" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1771280302" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1771276201" count="1">
+      <pm:colors xmlns:pm="smNativeData" id="1771280302" count="1">
         <pm:color name="Color 24" rgb="0070C0"/>
       </pm:colors>
     </ext>
@@ -3256,7 +3286,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1771276201" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1771280302" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -3265,14 +3295,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1771276201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1771276201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1771280302" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1771280302" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1771276201" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1771280302" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -3294,7 +3324,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1771276201" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1771280302" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -3303,14 +3333,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1771276201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1771276201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1771280302" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1771280302" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1771276201" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1771280302" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -3332,7 +3362,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1771276201" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1771280302" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -3341,14 +3371,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1771276201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1771276201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1771280302" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1771280302" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1771276201" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1771280302" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -3370,7 +3400,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1771276201" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1771280302" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -3379,14 +3409,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1771276201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1771276201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1771280302" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1771280302" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1771276201" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1771280302" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -3408,7 +3438,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1771276201" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1771280302" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -3417,14 +3447,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1771276201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1771276201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1771280302" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1771280302" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1771276201" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1771280302" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>